<commit_message>
.xlsx files import fixes
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/files/exported/expenses.xlsx
+++ b/src/main/webapp/resources/files/exported/expenses.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Audi A4 B6 1.8T" r:id="rId3" sheetId="1"/>
+    <sheet name="Suzuki SX4" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -50,9 +50,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Pierwsze badanie techniczne w kraju.</t>
-  </si>
-  <si>
     <t>Polisa OC</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>2020-02-24</t>
   </si>
   <si>
-    <t xml:space="preserve">MTU OC+NNW </t>
-  </si>
-  <si>
     <t>Pompka spryskiwacza</t>
   </si>
   <si>
@@ -74,18 +68,12 @@
     <t>2020-03-02</t>
   </si>
   <si>
-    <t>Pompka spryskiwacza reflektorów</t>
-  </si>
-  <si>
     <t>Żarówki</t>
   </si>
   <si>
     <t>Other</t>
   </si>
   <si>
-    <t>Żarówki świateł mijania Bosch Xenon Blue H7</t>
-  </si>
-  <si>
     <t>Rozrząd, olej, filtry</t>
   </si>
   <si>
@@ -95,52 +83,34 @@
     <t>2020-03-05</t>
   </si>
   <si>
-    <t>Zestaw rozrządu, pompa wody, pasek wielorowkowy, rolka napinacza paska, rolka prowadząca pasek, olej Castrol 5W30, filtr oleju, filtr kabinowy, płyn chłodniczy, zawór DV</t>
-  </si>
-  <si>
     <t xml:space="preserve">Świece </t>
   </si>
   <si>
     <t>2020-03-06</t>
   </si>
   <si>
-    <t>Świece NGK PRF6Q</t>
-  </si>
-  <si>
     <t>Wycieraczki</t>
   </si>
   <si>
     <t>2020-03-10</t>
   </si>
   <si>
-    <t xml:space="preserve">Wymiana wycieraczek </t>
-  </si>
-  <si>
     <t>Intercooler BEX</t>
   </si>
   <si>
     <t>2020-04-06</t>
   </si>
   <si>
-    <t>Montaż drugiego intercoolera</t>
-  </si>
-  <si>
     <t>Czujnik ECT</t>
   </si>
   <si>
     <t>2020-04-09</t>
   </si>
   <si>
-    <t>Wymiana czujnika temperatury cieczy chłodzącej</t>
-  </si>
-  <si>
     <t>Katalizator sportowy</t>
   </si>
   <si>
     <t>2020-04-28</t>
-  </si>
-  <si>
-    <t>Katalizator sportowy + montaż + złącze elastyczne + naprawa wydechu</t>
   </si>
   <si>
     <t>PB</t>
@@ -258,18 +228,18 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
       </c>
       <c r="D3" t="n">
         <v>105729.0</v>
@@ -284,18 +254,18 @@
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
       </c>
       <c r="D4" t="n">
         <v>106000.0</v>
@@ -310,18 +280,18 @@
         <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" t="n">
         <v>106000.0</v>
@@ -336,18 +306,18 @@
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D6" t="n">
         <v>106190.0</v>
@@ -362,18 +332,18 @@
         <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D7" t="n">
         <v>106250.0</v>
@@ -388,18 +358,18 @@
         <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D8" t="n">
         <v>106404.0</v>
@@ -414,18 +384,18 @@
         <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D9" t="n">
         <v>106660.0</v>
@@ -440,18 +410,18 @@
         <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D10" t="n">
         <v>106660.0</v>
@@ -466,18 +436,18 @@
         <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D11" t="n">
         <v>106900.0</v>
@@ -492,18 +462,18 @@
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D12" t="n">
         <v>105638.0</v>
@@ -523,13 +493,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D13" t="n">
         <v>105863.0</v>
@@ -549,13 +519,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D14" t="n">
         <v>105987.0</v>
@@ -575,13 +545,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D15" t="n">
         <v>106404.0</v>
@@ -601,13 +571,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D16" t="n">
         <v>106663.0</v>

</xml_diff>

<commit_message>
Remember Me function, 403 page.
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/files/exported/expenses.xlsx
+++ b/src/main/webapp/resources/files/exported/expenses.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Audi A4 B5" r:id="rId3" sheetId="1"/>
+    <sheet name="Audi A4 B6 1.8T" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -38,52 +38,109 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Świece</t>
+    <t>Badanie techniczne</t>
+  </si>
+  <si>
+    <t>MOT</t>
+  </si>
+  <si>
+    <t>2020-02-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Pierwsze badanie techniczne w kraju.</t>
+  </si>
+  <si>
+    <t>Polisa OC</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>2020-02-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTU OC+NNW </t>
+  </si>
+  <si>
+    <t>Pompka spryskiwacza</t>
+  </si>
+  <si>
+    <t>Repairs</t>
+  </si>
+  <si>
+    <t>2020-03-02</t>
+  </si>
+  <si>
+    <t>Pompka spryskiwacza reflektorów</t>
+  </si>
+  <si>
+    <t>Żarówki</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Żarówki świateł mijania Bosch Xenon Blue H7</t>
+  </si>
+  <si>
+    <t>Rozrząd, olej, filtry</t>
   </si>
   <si>
     <t>Exploitation</t>
   </si>
   <si>
-    <t>2016-12-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Wymiana świec</t>
-  </si>
-  <si>
-    <t>Osłona silnika</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>2016-12-17</t>
-  </si>
-  <si>
-    <t>Osłona silnika + montaż</t>
-  </si>
-  <si>
-    <t>Badanie techniczne</t>
-  </si>
-  <si>
-    <t>MOT</t>
-  </si>
-  <si>
-    <t>2017-12-27</t>
-  </si>
-  <si>
-    <t>Ubezpieczenie OC</t>
-  </si>
-  <si>
-    <t>Insurance</t>
-  </si>
-  <si>
-    <t>2017-12-15</t>
-  </si>
-  <si>
-    <t>PZU</t>
+    <t>2020-03-05</t>
+  </si>
+  <si>
+    <t>Zestaw rozrządu, pompa wody, pasek wielorowkowy, rolka napinacza paska, rolka prowadząca pasek, olej Castrol 5W30, filtr oleju, filtr kabinowy, płyn chłodniczy, zawór DV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Świece </t>
+  </si>
+  <si>
+    <t>2020-03-06</t>
+  </si>
+  <si>
+    <t>Świece NGK PRF6Q</t>
+  </si>
+  <si>
+    <t>Wycieraczki</t>
+  </si>
+  <si>
+    <t>2020-03-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wymiana wycieraczek </t>
+  </si>
+  <si>
+    <t>Intercooler BEX</t>
+  </si>
+  <si>
+    <t>2020-04-06</t>
+  </si>
+  <si>
+    <t>Montaż drugiego intercoolera</t>
+  </si>
+  <si>
+    <t>Czujnik ECT</t>
+  </si>
+  <si>
+    <t>2020-04-09</t>
+  </si>
+  <si>
+    <t>Wymiana czujnika temperatury cieczy chłodzącej</t>
+  </si>
+  <si>
+    <t>Katalizator sportowy</t>
+  </si>
+  <si>
+    <t>2020-04-28</t>
+  </si>
+  <si>
+    <t>Katalizator sportowy + montaż + złącze elastyczne + naprawa wydechu</t>
   </si>
   <si>
     <t>PB</t>
@@ -92,16 +149,16 @@
     <t>Fuel</t>
   </si>
   <si>
-    <t>2016-12-20</t>
-  </si>
-  <si>
-    <t>LPG</t>
-  </si>
-  <si>
-    <t>2016-12-27</t>
-  </si>
-  <si>
-    <t>2016-12-03</t>
+    <t>2020-02-15</t>
+  </si>
+  <si>
+    <t>2020-02-26</t>
+  </si>
+  <si>
+    <t>2020-02-27</t>
+  </si>
+  <si>
+    <t>2020-04-10</t>
   </si>
 </sst>
 </file>
@@ -146,7 +203,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -189,10 +246,10 @@
         <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>221768.0</v>
+        <v>105729.0</v>
       </c>
       <c r="E2" t="n">
-        <v>87.0</v>
+        <v>99.98999786376953</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -215,10 +272,10 @@
         <v>15</v>
       </c>
       <c r="D3" t="n">
-        <v>223848.0</v>
+        <v>105729.0</v>
       </c>
       <c r="E3" t="n">
-        <v>145.0</v>
+        <v>706.0</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -241,10 +298,10 @@
         <v>19</v>
       </c>
       <c r="D4" t="n">
-        <v>237720.0</v>
+        <v>106000.0</v>
       </c>
       <c r="E4" t="n">
-        <v>162.0</v>
+        <v>69.52999877929688</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -253,24 +310,24 @@
         <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D5" t="n">
-        <v>228391.0</v>
+        <v>106000.0</v>
       </c>
       <c r="E5" t="n">
-        <v>510.0</v>
+        <v>91.69999694824219</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -293,96 +350,278 @@
         <v>26</v>
       </c>
       <c r="D6" t="n">
-        <v>220536.0</v>
+        <v>106190.0</v>
       </c>
       <c r="E6" t="n">
-        <v>45.70000076293945</v>
-      </c>
-      <c r="F6" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>30.0</v>
+        <v>1400.0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" t="n">
-        <v>220942.0</v>
+        <v>106250.0</v>
       </c>
       <c r="E7" t="n">
-        <v>81.76000213623047</v>
-      </c>
-      <c r="F7" t="n">
-        <v>39.310001373291016</v>
-      </c>
-      <c r="G7" t="n">
-        <v>49.0</v>
+        <v>179.9600067138672</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D8" t="n">
-        <v>220942.0</v>
+        <v>106404.0</v>
       </c>
       <c r="E8" t="n">
-        <v>21.100000381469727</v>
-      </c>
-      <c r="F8" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>27.0</v>
+        <v>44.79999923706055</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D9" t="n">
-        <v>221318.0</v>
+        <v>106660.0</v>
       </c>
       <c r="E9" t="n">
-        <v>80.9800033569336</v>
-      </c>
-      <c r="F9" t="n">
-        <v>38.02000045776367</v>
-      </c>
-      <c r="G9" t="n">
-        <v>49.0</v>
+        <v>650.0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
       </c>
       <c r="H9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="n">
+        <v>106660.0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="n">
+        <v>106900.0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1175.0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="n">
+        <v>105638.0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>141.4199981689453</v>
+      </c>
+      <c r="F12" t="n">
+        <v>30.09000015258789</v>
+      </c>
+      <c r="G12" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="n">
+        <v>105863.0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>100.7699966430664</v>
+      </c>
+      <c r="F13" t="n">
+        <v>21.350000381469727</v>
+      </c>
+      <c r="G13" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="n">
+        <v>105987.0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>150.25999450683594</v>
+      </c>
+      <c r="F14" t="n">
+        <v>31.239999771118164</v>
+      </c>
+      <c r="G14" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="n">
+        <v>106404.0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>256.25</v>
+      </c>
+      <c r="F15" t="n">
+        <v>54.290000915527344</v>
+      </c>
+      <c r="G15" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="n">
+        <v>106663.0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>112.30999755859375</v>
+      </c>
+      <c r="F16" t="n">
+        <v>27.729999542236328</v>
+      </c>
+      <c r="G16" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="H16" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
User registration / login system, with Remember Me function. Several improvements.
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/files/exported/expenses.xlsx
+++ b/src/main/webapp/resources/files/exported/expenses.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -50,9 +50,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Pierwsze badanie techniczne w kraju.</t>
-  </si>
-  <si>
     <t>Polisa OC</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>2020-02-24</t>
   </si>
   <si>
-    <t xml:space="preserve">MTU OC+NNW </t>
-  </si>
-  <si>
     <t>Pompka spryskiwacza</t>
   </si>
   <si>
@@ -74,18 +68,12 @@
     <t>2020-03-02</t>
   </si>
   <si>
-    <t>Pompka spryskiwacza reflektorów</t>
-  </si>
-  <si>
     <t>Żarówki</t>
   </si>
   <si>
     <t>Other</t>
   </si>
   <si>
-    <t>Żarówki świateł mijania Bosch Xenon Blue H7</t>
-  </si>
-  <si>
     <t>Rozrząd, olej, filtry</t>
   </si>
   <si>
@@ -95,52 +83,61 @@
     <t>2020-03-05</t>
   </si>
   <si>
-    <t>Zestaw rozrządu, pompa wody, pasek wielorowkowy, rolka napinacza paska, rolka prowadząca pasek, olej Castrol 5W30, filtr oleju, filtr kabinowy, płyn chłodniczy, zawór DV</t>
-  </si>
-  <si>
     <t xml:space="preserve">Świece </t>
   </si>
   <si>
     <t>2020-03-06</t>
   </si>
   <si>
-    <t>Świece NGK PRF6Q</t>
-  </si>
-  <si>
     <t>Wycieraczki</t>
   </si>
   <si>
     <t>2020-03-10</t>
   </si>
   <si>
-    <t xml:space="preserve">Wymiana wycieraczek </t>
-  </si>
-  <si>
     <t>Intercooler BEX</t>
   </si>
   <si>
     <t>2020-04-06</t>
   </si>
   <si>
-    <t>Montaż drugiego intercoolera</t>
-  </si>
-  <si>
     <t>Czujnik ECT</t>
   </si>
   <si>
     <t>2020-04-09</t>
   </si>
   <si>
-    <t>Wymiana czujnika temperatury cieczy chłodzącej</t>
-  </si>
-  <si>
     <t>Katalizator sportowy</t>
   </si>
   <si>
     <t>2020-04-28</t>
   </si>
   <si>
-    <t>Katalizator sportowy + montaż + złącze elastyczne + naprawa wydechu</t>
+    <t>Chip tuning</t>
+  </si>
+  <si>
+    <t>2020-05-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K-Sport Opole. Zwiększenie mocy + montaż wtryskiwaczy + wyłączenie drugiej sondy lambda. </t>
+  </si>
+  <si>
+    <t>Tarcze i klocki hamulcowe przód</t>
+  </si>
+  <si>
+    <t>2020-05-15</t>
+  </si>
+  <si>
+    <t>Tarcze 312mm + klocki + jarzma + zaciski (niezamontowane)</t>
+  </si>
+  <si>
+    <t>Sprzęgło, uszczelnienie silnika i skrzyni, oleje</t>
+  </si>
+  <si>
+    <t>2020-06-16</t>
+  </si>
+  <si>
+    <t>- Sprzęgło komplet z dwumasą LUK 1.9 TDI AWX&lt;br&gt;- Uszczelnienie, czyszczenie miski olejowej&lt;br&gt;- Uszczelka pokrywy zaworów&lt;br&gt;- Olej w skrzyni RAVENOL TSG 75W90&lt;br&gt;- Olej w moście RAVENOL TGO 75W90&lt;br&gt;- Simering w skrzyni&lt;br&gt;- Osłona przegubu prawego wewnętrznego tył OEM&lt;br&gt;- Tarcze i klocki hamulcowe tył FEBI + TRW&lt;br&gt;- Śruby jarzm hamulcowych tył&lt;br&gt;- Czyszczenie i smarowanie przegubu prawego wewnętrznego tył&lt;br&gt;- Odpływ oleju z turbo</t>
   </si>
   <si>
     <t>PB</t>
@@ -159,6 +156,15 @@
   </si>
   <si>
     <t>2020-04-10</t>
+  </si>
+  <si>
+    <t>2020-05-08</t>
+  </si>
+  <si>
+    <t>2020-05-17</t>
+  </si>
+  <si>
+    <t>2020-06-25</t>
   </si>
 </sst>
 </file>
@@ -203,7 +209,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -258,18 +264,18 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
       </c>
       <c r="D3" t="n">
         <v>105729.0</v>
@@ -284,18 +290,18 @@
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
       </c>
       <c r="D4" t="n">
         <v>106000.0</v>
@@ -310,18 +316,18 @@
         <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" t="n">
         <v>106000.0</v>
@@ -336,18 +342,18 @@
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D6" t="n">
         <v>106190.0</v>
@@ -362,18 +368,18 @@
         <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D7" t="n">
         <v>106250.0</v>
@@ -388,18 +394,18 @@
         <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D8" t="n">
         <v>106404.0</v>
@@ -414,18 +420,18 @@
         <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D9" t="n">
         <v>106660.0</v>
@@ -440,18 +446,18 @@
         <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D10" t="n">
         <v>106660.0</v>
@@ -466,18 +472,18 @@
         <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D11" t="n">
         <v>106900.0</v>
@@ -492,108 +498,108 @@
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D12" t="n">
-        <v>105638.0</v>
+        <v>107300.0</v>
       </c>
       <c r="E12" t="n">
-        <v>141.4199981689453</v>
-      </c>
-      <c r="F12" t="n">
-        <v>30.09000015258789</v>
-      </c>
-      <c r="G12" t="n">
-        <v>33.0</v>
+        <v>1480.0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D13" t="n">
-        <v>105863.0</v>
+        <v>107350.0</v>
       </c>
       <c r="E13" t="n">
-        <v>100.7699966430664</v>
-      </c>
-      <c r="F13" t="n">
-        <v>21.350000381469727</v>
-      </c>
-      <c r="G13" t="n">
-        <v>33.0</v>
+        <v>360.0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D14" t="n">
-        <v>105987.0</v>
+        <v>107700.0</v>
       </c>
       <c r="E14" t="n">
-        <v>150.25999450683594</v>
-      </c>
-      <c r="F14" t="n">
-        <v>31.239999771118164</v>
-      </c>
-      <c r="G14" t="n">
-        <v>57.0</v>
+        <v>4220.0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
         <v>43</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>44</v>
       </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
       <c r="D15" t="n">
-        <v>106404.0</v>
+        <v>105638.0</v>
       </c>
       <c r="E15" t="n">
-        <v>256.25</v>
+        <v>141.4199981689453</v>
       </c>
       <c r="F15" t="n">
-        <v>54.290000915527344</v>
+        <v>30.09000015258789</v>
       </c>
       <c r="G15" t="n">
-        <v>66.0</v>
+        <v>33.0</v>
       </c>
       <c r="H15" t="s">
         <v>11</v>
@@ -601,27 +607,183 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
         <v>43</v>
       </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
       <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="n">
+        <v>105863.0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>100.7699966430664</v>
+      </c>
+      <c r="F16" t="n">
+        <v>21.350000381469727</v>
+      </c>
+      <c r="G16" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" t="n">
+        <v>105987.0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>150.25999450683594</v>
+      </c>
+      <c r="F17" t="n">
+        <v>31.239999771118164</v>
+      </c>
+      <c r="G17" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" t="n">
+        <v>106404.0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>256.25</v>
+      </c>
+      <c r="F18" t="n">
+        <v>54.290000915527344</v>
+      </c>
+      <c r="G18" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" t="n">
+        <v>106663.0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>112.30999755859375</v>
+      </c>
+      <c r="F19" t="n">
+        <v>27.729999542236328</v>
+      </c>
+      <c r="G19" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
         <v>48</v>
       </c>
-      <c r="D16" t="n">
-        <v>106663.0</v>
-      </c>
-      <c r="E16" t="n">
-        <v>112.30999755859375</v>
-      </c>
-      <c r="F16" t="n">
-        <v>27.729999542236328</v>
-      </c>
-      <c r="G16" t="n">
+      <c r="D20" t="n">
+        <v>107116.0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>203.3000030517578</v>
+      </c>
+      <c r="F20" t="n">
+        <v>53.63999938964844</v>
+      </c>
+      <c r="G20" t="n">
         <v>66.0</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" t="n">
+        <v>107661.0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>222.8300018310547</v>
+      </c>
+      <c r="F21" t="n">
+        <v>57.43000030517578</v>
+      </c>
+      <c r="G21" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="n">
+        <v>108242.0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>233.14999389648438</v>
+      </c>
+      <c r="F22" t="n">
+        <v>55.380001068115234</v>
+      </c>
+      <c r="G22" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="H22" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed validation of adding new vehicle and missing descriptions when importing from excel.
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/files/exported/expenses.xlsx
+++ b/src/main/webapp/resources/files/exported/expenses.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Audi A4 B6 1.8T" r:id="rId3" sheetId="1"/>
+    <sheet name="Audi Test" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -140,6 +140,33 @@
     <t>- Sprzęgło komplet z dwumasą LUK 1.9 TDI AWX&lt;br&gt;- Uszczelnienie, czyszczenie miski olejowej&lt;br&gt;- Uszczelka pokrywy zaworów&lt;br&gt;- Olej w skrzyni RAVENOL TSG 75W90&lt;br&gt;- Olej w moście RAVENOL TGO 75W90&lt;br&gt;- Simering w skrzyni&lt;br&gt;- Osłona przegubu prawego wewnętrznego tył OEM&lt;br&gt;- Tarcze i klocki hamulcowe tył FEBI + TRW&lt;br&gt;- Śruby jarzm hamulcowych tył&lt;br&gt;- Czyszczenie i smarowanie przegubu prawego wewnętrznego tył&lt;br&gt;- Odpływ oleju z turbo</t>
   </si>
   <si>
+    <t>Przeguby wewnętrzne przód</t>
+  </si>
+  <si>
+    <t>2020-07-21</t>
+  </si>
+  <si>
+    <t>Przeguby wewnętrzne SKF + montaż</t>
+  </si>
+  <si>
+    <t>Przegląd klimatyzacji</t>
+  </si>
+  <si>
+    <t>2020-07-27</t>
+  </si>
+  <si>
+    <t>Uzupełniono 90g czynnika</t>
+  </si>
+  <si>
+    <t>Podpora wału</t>
+  </si>
+  <si>
+    <t>2020-08-13</t>
+  </si>
+  <si>
+    <t>Podpora wału z łożyskiem FAG + wymiana</t>
+  </si>
+  <si>
     <t>PB</t>
   </si>
   <si>
@@ -165,6 +192,27 @@
   </si>
   <si>
     <t>2020-06-25</t>
+  </si>
+  <si>
+    <t>2020-07-20</t>
+  </si>
+  <si>
+    <t>2020-07-29</t>
+  </si>
+  <si>
+    <t>2020-08-17</t>
+  </si>
+  <si>
+    <t>2020-09-03</t>
+  </si>
+  <si>
+    <t>2020-09-06</t>
+  </si>
+  <si>
+    <t>2020-09-15</t>
+  </si>
+  <si>
+    <t>2020-09-24</t>
   </si>
 </sst>
 </file>
@@ -209,7 +257,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -584,100 +632,100 @@
         <v>42</v>
       </c>
       <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
         <v>43</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="n">
+        <v>108800.0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>520.0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s">
         <v>44</v>
-      </c>
-      <c r="D15" t="n">
-        <v>105638.0</v>
-      </c>
-      <c r="E15" t="n">
-        <v>141.4199981689453</v>
-      </c>
-      <c r="F15" t="n">
-        <v>30.09000015258789</v>
-      </c>
-      <c r="G15" t="n">
-        <v>33.0</v>
-      </c>
-      <c r="H15" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D16" t="n">
-        <v>105863.0</v>
+        <v>109000.0</v>
       </c>
       <c r="E16" t="n">
-        <v>100.7699966430664</v>
-      </c>
-      <c r="F16" t="n">
-        <v>21.350000381469727</v>
-      </c>
-      <c r="G16" t="n">
-        <v>33.0</v>
+        <v>79.0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
       </c>
       <c r="H16" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D17" t="n">
-        <v>105987.0</v>
+        <v>109500.0</v>
       </c>
       <c r="E17" t="n">
-        <v>150.25999450683594</v>
-      </c>
-      <c r="F17" t="n">
-        <v>31.239999771118164</v>
-      </c>
-      <c r="G17" t="n">
-        <v>57.0</v>
+        <v>450.0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
       </c>
       <c r="H17" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="D18" t="n">
-        <v>106404.0</v>
+        <v>105638.0</v>
       </c>
       <c r="E18" t="n">
-        <v>256.25</v>
+        <v>141.4199981689453</v>
       </c>
       <c r="F18" t="n">
-        <v>54.290000915527344</v>
+        <v>30.09000015258789</v>
       </c>
       <c r="G18" t="n">
-        <v>66.0</v>
+        <v>33.0</v>
       </c>
       <c r="H18" t="s">
         <v>11</v>
@@ -685,25 +733,25 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D19" t="n">
-        <v>106663.0</v>
+        <v>105863.0</v>
       </c>
       <c r="E19" t="n">
-        <v>112.30999755859375</v>
+        <v>100.7699966430664</v>
       </c>
       <c r="F19" t="n">
-        <v>27.729999542236328</v>
+        <v>21.350000381469727</v>
       </c>
       <c r="G19" t="n">
-        <v>66.0</v>
+        <v>33.0</v>
       </c>
       <c r="H19" t="s">
         <v>11</v>
@@ -711,25 +759,25 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D20" t="n">
-        <v>107116.0</v>
+        <v>105987.0</v>
       </c>
       <c r="E20" t="n">
-        <v>203.3000030517578</v>
+        <v>150.25999450683594</v>
       </c>
       <c r="F20" t="n">
-        <v>53.63999938964844</v>
+        <v>31.239999771118164</v>
       </c>
       <c r="G20" t="n">
-        <v>66.0</v>
+        <v>57.0</v>
       </c>
       <c r="H20" t="s">
         <v>11</v>
@@ -737,22 +785,22 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="D21" t="n">
-        <v>107661.0</v>
+        <v>106404.0</v>
       </c>
       <c r="E21" t="n">
-        <v>222.8300018310547</v>
+        <v>256.25</v>
       </c>
       <c r="F21" t="n">
-        <v>57.43000030517578</v>
+        <v>54.290000915527344</v>
       </c>
       <c r="G21" t="n">
         <v>66.0</v>
@@ -763,27 +811,313 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D22" t="n">
+        <v>106663.0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>112.30999755859375</v>
+      </c>
+      <c r="F22" t="n">
+        <v>27.729999542236328</v>
+      </c>
+      <c r="G22" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" t="n">
+        <v>107116.0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>203.3000030517578</v>
+      </c>
+      <c r="F23" t="n">
+        <v>53.63999938964844</v>
+      </c>
+      <c r="G23" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" t="n">
+        <v>107661.0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>222.8300018310547</v>
+      </c>
+      <c r="F24" t="n">
+        <v>57.43000030517578</v>
+      </c>
+      <c r="G24" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" t="n">
         <v>108242.0</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E25" t="n">
         <v>233.14999389648438</v>
       </c>
-      <c r="F22" t="n">
+      <c r="F25" t="n">
         <v>55.380001068115234</v>
       </c>
-      <c r="G22" t="n">
-        <v>66.0</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="G25" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" t="n">
+        <v>108686.0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>203.3000030517578</v>
+      </c>
+      <c r="F26" t="n">
+        <v>47.279998779296875</v>
+      </c>
+      <c r="G26" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" t="n">
+        <v>109242.0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>225.3000030517578</v>
+      </c>
+      <c r="F27" t="n">
+        <v>50.290000915527344</v>
+      </c>
+      <c r="G27" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="H27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" t="n">
+        <v>109761.0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>225.72000122070312</v>
+      </c>
+      <c r="F28" t="n">
+        <v>52.0099983215332</v>
+      </c>
+      <c r="G28" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="H28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" t="n">
+        <v>110194.0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>188.85000610351562</v>
+      </c>
+      <c r="F29" t="n">
+        <v>42.060001373291016</v>
+      </c>
+      <c r="G29" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="H29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" t="n">
+        <v>110635.0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>187.38999938964844</v>
+      </c>
+      <c r="F30" t="n">
+        <v>42.29999923706055</v>
+      </c>
+      <c r="G30" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" t="n">
+        <v>111011.0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>160.1699981689453</v>
+      </c>
+      <c r="F31" t="n">
+        <v>36.9900016784668</v>
+      </c>
+      <c r="G31" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="H31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" t="n">
+        <v>111431.0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>184.0399932861328</v>
+      </c>
+      <c r="F32" t="n">
+        <v>41.08000183105469</v>
+      </c>
+      <c r="G32" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="H32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" t="n">
+        <v>111669.0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>114.08999633789062</v>
+      </c>
+      <c r="F33" t="n">
+        <v>24.1200008392334</v>
+      </c>
+      <c r="G33" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="H33" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added PWA (manifest.json, service-worker.js), delete of expense confirmation, bug fixes.
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/files/exported/expenses.xlsx
+++ b/src/main/webapp/resources/files/exported/expenses.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Audi Test" r:id="rId3" sheetId="1"/>
+    <sheet name="Audi A4 B6" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -119,54 +119,36 @@
     <t>2020-05-12</t>
   </si>
   <si>
-    <t xml:space="preserve">K-Sport Opole. Zwiększenie mocy + montaż wtryskiwaczy + wyłączenie drugiej sondy lambda. </t>
-  </si>
-  <si>
     <t>Tarcze i klocki hamulcowe przód</t>
   </si>
   <si>
     <t>2020-05-15</t>
   </si>
   <si>
-    <t>Tarcze 312mm + klocki + jarzma + zaciski (niezamontowane)</t>
-  </si>
-  <si>
     <t>Sprzęgło, uszczelnienie silnika i skrzyni, oleje</t>
   </si>
   <si>
     <t>2020-06-16</t>
   </si>
   <si>
-    <t>- Sprzęgło komplet z dwumasą LUK 1.9 TDI AWX&lt;br&gt;- Uszczelnienie, czyszczenie miski olejowej&lt;br&gt;- Uszczelka pokrywy zaworów&lt;br&gt;- Olej w skrzyni RAVENOL TSG 75W90&lt;br&gt;- Olej w moście RAVENOL TGO 75W90&lt;br&gt;- Simering w skrzyni&lt;br&gt;- Osłona przegubu prawego wewnętrznego tył OEM&lt;br&gt;- Tarcze i klocki hamulcowe tył FEBI + TRW&lt;br&gt;- Śruby jarzm hamulcowych tył&lt;br&gt;- Czyszczenie i smarowanie przegubu prawego wewnętrznego tył&lt;br&gt;- Odpływ oleju z turbo</t>
-  </si>
-  <si>
     <t>Przeguby wewnętrzne przód</t>
   </si>
   <si>
     <t>2020-07-21</t>
   </si>
   <si>
-    <t>Przeguby wewnętrzne SKF + montaż</t>
-  </si>
-  <si>
     <t>Przegląd klimatyzacji</t>
   </si>
   <si>
     <t>2020-07-27</t>
   </si>
   <si>
-    <t>Uzupełniono 90g czynnika</t>
-  </si>
-  <si>
     <t>Podpora wału</t>
   </si>
   <si>
     <t>2020-08-13</t>
   </si>
   <si>
-    <t>Podpora wału z łożyskiem FAG + wymiana</t>
-  </si>
-  <si>
     <t>PB</t>
   </si>
   <si>
@@ -210,9 +192,6 @@
   </si>
   <si>
     <t>2020-09-15</t>
-  </si>
-  <si>
-    <t>2020-09-24</t>
   </si>
 </sst>
 </file>
@@ -257,7 +236,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -572,18 +551,18 @@
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" t="n">
         <v>107350.0</v>
@@ -598,18 +577,18 @@
         <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D14" t="n">
         <v>107700.0</v>
@@ -624,18 +603,18 @@
         <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D15" t="n">
         <v>108800.0</v>
@@ -650,18 +629,18 @@
         <v>11</v>
       </c>
       <c r="H15" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D16" t="n">
         <v>109000.0</v>
@@ -676,18 +655,18 @@
         <v>11</v>
       </c>
       <c r="H16" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D17" t="n">
         <v>109500.0</v>
@@ -702,18 +681,18 @@
         <v>11</v>
       </c>
       <c r="H17" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D18" t="n">
         <v>105638.0</v>
@@ -733,13 +712,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D19" t="n">
         <v>105863.0</v>
@@ -759,13 +738,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D20" t="n">
         <v>105987.0</v>
@@ -785,10 +764,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
         <v>26</v>
@@ -811,13 +790,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D22" t="n">
         <v>106663.0</v>
@@ -837,13 +816,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
         <v>51</v>
-      </c>
-      <c r="B23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" t="s">
-        <v>57</v>
       </c>
       <c r="D23" t="n">
         <v>107116.0</v>
@@ -863,13 +842,13 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
         <v>52</v>
-      </c>
-      <c r="C24" t="s">
-        <v>58</v>
       </c>
       <c r="D24" t="n">
         <v>107661.0</v>
@@ -889,13 +868,13 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D25" t="n">
         <v>108242.0</v>
@@ -915,13 +894,13 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D26" t="n">
         <v>108686.0</v>
@@ -941,13 +920,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D27" t="n">
         <v>109242.0</v>
@@ -967,13 +946,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D28" t="n">
         <v>109761.0</v>
@@ -993,13 +972,13 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D29" t="n">
         <v>110194.0</v>
@@ -1019,13 +998,13 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D30" t="n">
         <v>110635.0</v>
@@ -1045,13 +1024,13 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D31" t="n">
         <v>111011.0</v>
@@ -1066,58 +1045,6 @@
         <v>66.0</v>
       </c>
       <c r="H31" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" t="s">
-        <v>52</v>
-      </c>
-      <c r="C32" t="s">
-        <v>66</v>
-      </c>
-      <c r="D32" t="n">
-        <v>111431.0</v>
-      </c>
-      <c r="E32" t="n">
-        <v>184.0399932861328</v>
-      </c>
-      <c r="F32" t="n">
-        <v>41.08000183105469</v>
-      </c>
-      <c r="G32" t="n">
-        <v>66.0</v>
-      </c>
-      <c r="H32" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>51</v>
-      </c>
-      <c r="B33" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" t="s">
-        <v>66</v>
-      </c>
-      <c r="D33" t="n">
-        <v>111669.0</v>
-      </c>
-      <c r="E33" t="n">
-        <v>114.08999633789062</v>
-      </c>
-      <c r="F33" t="n">
-        <v>24.1200008392334</v>
-      </c>
-      <c r="G33" t="n">
-        <v>66.0</v>
-      </c>
-      <c r="H33" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>